<commit_message>
add Stanislaus County for CAMH region
</commit_message>
<xml_diff>
--- a/parameters/Local/CAMH-2020-Parameters.xlsx
+++ b/parameters/Local/CAMH-2020-Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/automatingcbc/parameters/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F6B48F-BD08-184C-8DDE-7C34CFCB1EEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7635FA-C2CC-AE4C-8000-F805F4380249}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29680" yWindow="3920" windowWidth="27320" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>CircleLongitude</t>
   </si>
   <si>
-    <t>US-CA-085</t>
-  </si>
-  <si>
     <t>eBirdRegion</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>CAMH</t>
+  </si>
+  <si>
+    <t>US-CA-085,US-CA-099</t>
   </si>
 </sst>
 </file>
@@ -943,7 +943,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1000,31 +1000,31 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>90</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>44198</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>44198</v>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>